<commit_message>
Reorganisation and adding interpolation method to feature matrix
</commit_message>
<xml_diff>
--- a/feature-matrix/deformation-model-feature-matrix.xlsx
+++ b/feature-matrix/deformation-model-feature-matrix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24004"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F73B4A2-6E86-4C77-A81F-00E8DCD2D019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FC9FB73-B384-4ADF-ACA7-80C6857B3FB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C54" authorId="1" shapeId="0" xr:uid="{8F935A96-4B21-4011-8A9B-ADACA425754F}">
+    <comment ref="C28" authorId="1" shapeId="0" xr:uid="{8F935A96-4B21-4011-8A9B-ADACA425754F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
   <si>
     <t>Deformation model functional model feature analysis</t>
   </si>
@@ -105,6 +105,9 @@
     <t>Redundant</t>
   </si>
   <si>
+    <t>Undesirable</t>
+  </si>
+  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -171,6 +174,69 @@
     <t>Explicity defined formulae for all calculations</t>
   </si>
   <si>
+    <t>Deformation parametsrs</t>
+  </si>
+  <si>
+    <t>Displacement in metres E/N/U</t>
+  </si>
+  <si>
+    <t>Displacement in source CRS units</t>
+  </si>
+  <si>
+    <t>Displacement in other units (eg seconds, mm?)</t>
+  </si>
+  <si>
+    <t>Uncertainty in metres</t>
+  </si>
+  <si>
+    <t>Uncertainty in source CRS units</t>
+  </si>
+  <si>
+    <t>Uncertainty in other units</t>
+  </si>
+  <si>
+    <t>Options for confidence level/SE multiplier</t>
+  </si>
+  <si>
+    <t>Eg 2SE, 95% confidence</t>
+  </si>
+  <si>
+    <t>Horizontal/vertical uncertainty at each node</t>
+  </si>
+  <si>
+    <t>Horizontal covariance</t>
+  </si>
+  <si>
+    <t>May be just independent E/N uncertainty</t>
+  </si>
+  <si>
+    <t>Full covariance at nodes</t>
+  </si>
+  <si>
+    <t>No-data values</t>
+  </si>
+  <si>
+    <t>Quality alert flag at nodes</t>
+  </si>
+  <si>
+    <t>Flag indicating likely local quality issues (eg area affected by surface faulting)</t>
+  </si>
+  <si>
+    <t>Producer defined additional node parameters (ignored)</t>
+  </si>
+  <si>
+    <t>Displacment simply added to E/N/U coordinates</t>
+  </si>
+  <si>
+    <t>Note - may require scaling metres to degrees</t>
+  </si>
+  <si>
+    <t>Displacement added in local topocentric system</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Spatial model</t>
   </si>
   <si>
@@ -198,13 +264,22 @@
     <t>Rotated grids</t>
   </si>
   <si>
+    <t>Bilinear interpolation</t>
+  </si>
+  <si>
+    <t>Bicubic interpolation</t>
+  </si>
+  <si>
+    <t>"Geocentric bilinear" interplation</t>
+  </si>
+  <si>
     <t>Trianglated network models</t>
   </si>
   <si>
     <t>Note: Survey has only identified one deformation model is using triangulated network</t>
   </si>
   <si>
-    <t>14(15) parameter bursa wolf transformation</t>
+    <t>14(15) parameter Bursa-Wolf transformation</t>
   </si>
   <si>
     <t>Note: this has an implied time function</t>
@@ -216,36 +291,6 @@
     <t xml:space="preserve">Okada (1985) rectangular fault model </t>
   </si>
   <si>
-    <t>Deformation in source CRS units</t>
-  </si>
-  <si>
-    <t>Deformation in metres</t>
-  </si>
-  <si>
-    <t>Deformation in other units (eg seconds, mm?)</t>
-  </si>
-  <si>
-    <t>Uncertainty in source CRS units</t>
-  </si>
-  <si>
-    <t>Uncertainty in other units</t>
-  </si>
-  <si>
-    <t>Uncertainty in metres</t>
-  </si>
-  <si>
-    <t>No-data values</t>
-  </si>
-  <si>
-    <t>Quality alert flag at nodes</t>
-  </si>
-  <si>
-    <t>Flag indicating likely local quality issues (eg area affected by surface faulting)</t>
-  </si>
-  <si>
-    <t>Producer defined additional node parameters (ignored)</t>
-  </si>
-  <si>
     <t>Temporal model</t>
   </si>
   <si>
@@ -276,31 +321,7 @@
     <t>Cyclic function</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Composite function</t>
-  </si>
-  <si>
-    <t>Uncertainty representation</t>
-  </si>
-  <si>
-    <t>Options for confidence level/SE multiplier</t>
-  </si>
-  <si>
-    <t>Eg 2SE, 95% confidence</t>
-  </si>
-  <si>
-    <t>Horizontal/vertical uncertainty at each node</t>
-  </si>
-  <si>
-    <t>Horizontal covariance</t>
-  </si>
-  <si>
-    <t>(Simpler would be east/north uncertainty)</t>
-  </si>
-  <si>
-    <t>Full covariance at nodes</t>
   </si>
 </sst>
 </file>
@@ -352,9 +373,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -363,6 +381,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -687,7 +708,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="C54" dT="2021-04-09T02:45:42.21" personId="{045B2A42-21AC-40E5-841A-7D228C5EDA30}" id="{8F935A96-4B21-4011-8A9B-ADACA425754F}">
+  <threadedComment ref="C28" dT="2021-04-09T02:45:42.21" personId="{045B2A42-21AC-40E5-841A-7D228C5EDA30}" id="{8F935A96-4B21-4011-8A9B-ADACA425754F}">
     <text>Medium as combination of components more complex</text>
   </threadedComment>
 </ThreadedComments>
@@ -695,34 +716,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="52.28515625" customWidth="1"/>
-    <col min="2" max="3" width="11.5703125" style="5"/>
-    <col min="4" max="7" width="11.5703125" style="1"/>
-    <col min="8" max="8" width="65.85546875" customWidth="1"/>
+    <col min="2" max="3" width="11.5703125" style="4"/>
+    <col min="4" max="8" width="11.5703125" style="1"/>
+    <col min="9" max="9" width="65.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1">
+    <row r="3" spans="1:9" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="8" t="s">
@@ -731,542 +752,604 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>14</v>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+        <v>35</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="B23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="C25" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
+      <c r="C26" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
+      <c r="C27" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="C28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" t="s">
+      <c r="C29" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" t="s">
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" t="s">
+      <c r="C31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
+      <c r="B32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
+      <c r="B34" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
         <v>51</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
+      <c r="B35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
+      <c r="C35" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H37" t="s">
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
+      <c r="B38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="3" t="s">
+      <c r="B39" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="B40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="C41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>60</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>60</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>62</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>63</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>62</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>64</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>64</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" t="s">
         <v>65</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="B46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="3" t="s">
+      <c r="C49" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="s">
+    <row r="50" spans="1:9">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="C50" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" t="s">
+      <c r="B51" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" t="s">
+      <c r="C54" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" t="s">
+      <c r="B55" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>20</v>
+      <c r="B56" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="D3:H3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>